<commit_message>
Added google voice sample code, ppt material and port id for connection
</commit_message>
<xml_diff>
--- a/Sage X3 Hackathon instances and Teams.xlsx
+++ b/Sage X3 Hackathon instances and Teams.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lynsey.scott\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspaces\Hackathon\sage-x3-hackathon-2016\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11616"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
   <si>
     <t>Name</t>
   </si>
@@ -204,12 +204,15 @@
   </si>
   <si>
     <t>P@rtners_2016$</t>
+  </si>
+  <si>
+    <t>http://52.208.232.164:8124</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -580,24 +583,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
-    <col min="2" max="2" width="59.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" customWidth="1"/>
+    <col min="2" max="2" width="59.5546875" customWidth="1"/>
+    <col min="3" max="3" width="17.88671875" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="28.109375" customWidth="1"/>
     <col min="7" max="7" width="16" customWidth="1"/>
     <col min="8" max="8" width="57" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -623,7 +626,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -649,7 +652,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -675,7 +678,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -701,7 +704,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -727,7 +730,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -753,7 +756,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -779,7 +782,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -805,7 +808,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -822,19 +825,24 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>